<commit_message>
Added New Projects Data
</commit_message>
<xml_diff>
--- a/project-inventory-manzot-singh.xlsx
+++ b/project-inventory-manzot-singh.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="34">
   <si>
     <t xml:space="preserve">Project Inventory – Manjot Singh</t>
   </si>
@@ -46,6 +46,21 @@
     <t xml:space="preserve">Uploaded on Github (Yes/No)</t>
   </si>
   <si>
+    <t xml:space="preserve">3D Action RPG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unity3D (C#)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Work In Progress Action RPG game with top down persepective. Many features like Inventory, Quests, Menus, Data Serilization, Stamina System, NPC interactions have been done. But still remaining so much more to do.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
     <t xml:space="preserve">Grapplu -The Beginning</t>
   </si>
   <si>
@@ -55,15 +70,15 @@
     <t xml:space="preserve">2D Platfomer game made in Unity with features like Grapple Hook, Time slow, Time Rewind, 3 types of enemies, 2 Bosses, 2 levels</t>
   </si>
   <si>
-    <t xml:space="preserve">Yes</t>
+    <t xml:space="preserve">Movolit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Strategy based multi-Level 2D puzzle Game, with a dark and Challenging Environment. 2D Dynamic Lights and Shaders used in real time environment.</t>
   </si>
   <si>
     <t xml:space="preserve">Air Raid</t>
   </si>
   <si>
-    <t xml:space="preserve">Unity3D (C#)</t>
-  </si>
-  <si>
     <t xml:space="preserve">3D Airplane Simulator Game where you have to save the city flooded by enemies using a airplane that has different types of abilities such as shooting, throwing bombs,turrets,missiles and much more.</t>
   </si>
   <si>
@@ -80,9 +95,6 @@
   </si>
   <si>
     <t xml:space="preserve"> No</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No</t>
   </si>
   <si>
     <t xml:space="preserve">The Legend of Link</t>
@@ -119,7 +131,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -202,6 +214,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -351,7 +368,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -373,6 +390,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -469,17 +494,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A4:F29"/>
+  <dimension ref="A4:F31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.58"/>
@@ -487,7 +512,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="27.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -537,7 +561,7 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="92.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
@@ -548,170 +572,194 @@
         <v>10</v>
       </c>
       <c r="D10" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="81.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="B11" s="6" t="s">
         <v>14</v>
       </c>
+      <c r="C11" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="D11" s="4" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="69.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="D12" s="4" t="n">
         <v>2</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="81.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>18</v>
+      <c r="C13" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="D13" s="4" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="6" t="s">
+      <c r="D14" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="4" t="n">
+      <c r="B15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="E14" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="6" t="s">
+      <c r="E15" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="D15" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>11</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="104.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>27</v>
-      </c>
       <c r="D16" s="4" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="103.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="6" t="s">
+      <c r="D17" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="104.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="4" t="n">
+      <c r="B18" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="103.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
+      <c r="E19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4"/>
@@ -792,6 +840,22 @@
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>